<commit_message>
método get aplicado, avanza favorablemente
</commit_message>
<xml_diff>
--- a/src/results.xlsx
+++ b/src/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,175 +436,250 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>TÍTULO</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>DESCRIPCIÓN</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>released</t>
+          <t>REFERENCIA</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>notes</t>
+          <t>PRECIO</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>barcode</t>
+          <t>ISBN</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>matrix</t>
+          <t>SECCIÓN</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>format</t>
+          <t>ESTADO</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>DESCRIPCIÓN DEL ESTADO</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>OPERACIÓN</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>STOCK</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA DE PUBLICACIÓN</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>FORMA DE ENVÍO</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>GASTOS FIJOS</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Confusa E Felice</t>
+          <t>Carmen Consoli - Confusa E Felice CD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Made in the EU.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+          <t>Carmen Consoli - Confusa E Felice
+CD, Album,
+Italy, 
+Cat. No:
+Barcode: None</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>07314 537 179-2 01 / 51292784</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>07314 537 179-2 01 / 51292784</t>
+          <t>453</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Envíos muy rápidos con tarifa plana, combine discos y pague solo por el primer lote.</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Carmen Consoli</t>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>hoy</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>4,5</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Preguntas Y Flores</t>
+          <t>Cómplices - Preguntas Y Flores CD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Cómplices - Preguntas Y Flores
+CD, Album,
+Spain, 1993
+Cat. No:
+Barcode: 743211738828</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>7 43211 73882 8</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7 43211 73882 8</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>453</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>1993</v>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Envíos muy rápidos con tarifa plana, combine discos y pague solo por el primer lote.</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Cómplices</t>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>hoy</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>4,5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dance Into The Light</t>
+          <t>Phil Collins - Dance Into The Light CD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Phil Collins - Dance Into The Light
+CD, Album,
+Europe, 1996-10-14
+Cat. No:
+Barcode: 706301600023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1996-10-14</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Packaged in jewel case with transparent tray.
-Booklet: 16 pages, with lyrics
-℗ 1996 Philip Collins Ltd. Exclusively licensed to Atlantic Recording Corporation for the U.S. and WEA International Inc. for the rest of the world.
-© 1996 Atlantic Recording Corporation for the U.S. and WEA International Inc. for the rest of the world.
-All songs published by © 1996 Philip Collins Ltd/Hit &amp; Run ® Music (Publishing) Ltd except The Times They Are A-Changin' by Special Rider Music/Sony/ATV Music Publishing.
-Made in Germany by Warner Music Manufacturing Europe. A Time Warner Company.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
           <t>706301600023</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>063016000-2.2 WME</t>
+          <t>453</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>1996</v>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Envíos muy rápidos con tarifa plana, combine discos y pague solo por el primer lote.</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Phil Collins</t>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>hoy</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4,5</t>
         </is>
       </c>
     </row>

</xml_diff>